<commit_message>
Voeg secties over naamvallen toe
</commit_message>
<xml_diff>
--- a/questions_and_answers_ch2.xlsx
+++ b/questions_and_answers_ch2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5507553\Documents\GitHub\LesboekOekraiensNederlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFB5D949-B98A-4E50-BAEF-021632459A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F98C7-2BAC-4C44-88B7-11C3F336B3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DACCA6F-7BC7-4175-961A-DD307BF25DE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DACCA6F-7BC7-4175-961A-DD307BF25DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,169 +38,169 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
-    <t xml:space="preserve">  "Hoe zeg je 'hallo' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'tot ziens' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'alstublieft' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'ik' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'jij' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'hij' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'zij (vrouwelijk)' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe zeg je 'het' in het Oekraïens?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Привіт' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Добрий ранок' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Добрий день' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Добрий вечір' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Добраніч' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Бувайте' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'До побачення' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Будь ласка' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Дякую' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Вибачте' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Немає проблем' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Як справи?' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Добре' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'Згода' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'я' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'ти' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'він' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'вона' in het Nederlands?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Wat betekent 'воно' in het Nederlands?"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Привіт",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "До побачення",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Будь ласка",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "я",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "ти",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "він",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "вона",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "воно",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hallo",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Goedemorgen",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Goedemiddag",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Goede avond",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Goede nacht",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Tot ziens",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Alstublieft",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Dank u",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Sorry",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Geen probleem",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Hoe gaat het?",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Goed",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Akkoord",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "ik",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "jij",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "hij",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "zij (vrouwelijk)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "het"</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'воно' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  het</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'hallo' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Привіт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'tot ziens' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  До побачення</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'alstublieft' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Будь ласка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'ik' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  я</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'jij' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ти</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'hij' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  він</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'zij (vrouwelijk)' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  вона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe zeg je 'het' in het Oekraïens?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  воно</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Привіт' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Добрий ранок' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Goedemorgen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Добрий день' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Goedemiddag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Добрий вечір' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Goede avond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Добраніч' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Goede nacht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Бувайте' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tot ziens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'До побачення' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Будь ласка' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Alstublieft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Дякую' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dank u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Вибачте' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sorry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Немає проблем' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Geen probleem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Як справи?' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hoe gaat het?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Добре' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Goed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'Згода' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Akkoord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'я' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'ти' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  jij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'він' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  hij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wat betekent 'вона' in het Nederlands?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  zij (vrouwelijk)</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,191 +565,191 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -757,34 +757,34 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>